<commit_message>
1.2 version. Added helpMessages, logger, fixed saves bugs, added tests
</commit_message>
<xml_diff>
--- a/src/main/resources/test/test.xlsx
+++ b/src/main/resources/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreyserebryanskiy/IdeaProjects/badgeGenerator/src/test/testResources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreyserebryanskiy/IdeaProjects/badgeGenerator/src/main/resources/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,10 +72,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,13 +114,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,7 +419,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,5 +478,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>